<commit_message>
Demo thử web api sử dụng RestAPI
</commit_message>
<xml_diff>
--- a/Cac_cong_nghe_su_dung.xlsx
+++ b/Cac_cong_nghe_su_dung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\ASP.NET Project\Cars_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FDF000E-8540-4B26-93E8-DE1712A2A0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA7DBB-3E84-4641-9AB5-7BE097DFE68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58F966C1-4917-479B-8CB8-995AE431CB49}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>SignalR</t>
   </si>
   <si>
-    <t>Chat inbox giữa staff và customer, set unread, mark as read</t>
+    <t>Chat inbox giữa staff và customer, set unread, mark as read.</t>
   </si>
 </sst>
 </file>

</xml_diff>